<commit_message>
added racha from last 5 games
</commit_message>
<xml_diff>
--- a/TorneoApertura2016/week2.xlsx
+++ b/TorneoApertura2016/week2.xlsx
@@ -279,7 +279,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -330,6 +330,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -348,9 +356,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -362,7 +371,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -696,7 +706,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="A3" sqref="A3:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1273,6 +1283,7 @@
     <hyperlink ref="A3" r:id="rId9" display="Pachuca"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>